<commit_message>
Extracted products based on committment
</commit_message>
<xml_diff>
--- a/backend/data/ingredients.xlsx
+++ b/backend/data/ingredients.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cleanify-app\backend\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C7B21A-A22C-45D8-99B1-F1A14647AF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Skin type</t>
   </si>
@@ -89,43 +99,98 @@
   </si>
   <si>
     <t>• Vitamin C• Alpha Hydroxy Acids (AHAs)• Niacinamide• Hyaluronic Acid• Rosehip Oil• Antioxidants• Saffron Extract• Turmeric Extract</t>
+  </si>
+  <si>
+    <t>Product Suggestion AM</t>
+  </si>
+  <si>
+    <t>Product Suggestion PM</t>
+  </si>
+  <si>
+    <t>Commitment Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intensive </t>
+  </si>
+  <si>
+    <t>•Facewash
+•Moisturiser
+•Sunscreen</t>
+  </si>
+  <si>
+    <t>•Facewash
+•Antioxidant serum (like Vitamin C)
+•Moisturizer
+•Sunscreen</t>
+  </si>
+  <si>
+    <t>•Facewash
+•Toner (hydrating/exfoliating)
+•Essence
+•Antioxidant serum (Vitamin C)
+•Moisturizer
+•Sunscreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•Facewash
+•Serum/ Moisturiser
+</t>
+  </si>
+  <si>
+    <t>•Facewash
+•Treatment serum 
+(e.g., niacinamide, hyaluronic acid)
+•Moisturizer</t>
+  </si>
+  <si>
+    <t>•Cleanse
+•Toner
+•Active serum (AHA/BHA, retinol, peptides, etc.)
+•Hydrating serum (hyaluronic acid)
+•Moisturizer or sleeping mask</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -135,59 +200,58 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -377,27 +441,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.13"/>
-    <col customWidth="1" min="2" max="2" width="26.0"/>
-    <col customWidth="1" min="3" max="3" width="15.88"/>
-    <col customWidth="1" min="4" max="4" width="22.25"/>
-    <col customWidth="1" min="5" max="5" width="103.13"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" customWidth="1"/>
+    <col min="5" max="5" width="103.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -431,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -448,7 +515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -465,7 +532,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -482,7 +549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -499,7 +566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -516,7 +583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -533,7 +600,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -550,7 +617,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -567,21 +634,89 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>